<commit_message>
adding all kinds of new things from day 1 of the anc4 pilot
</commit_message>
<xml_diff>
--- a/data-general/ChlamEE_Treatments.xlsx
+++ b/data-general/ChlamEE_Treatments.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Abteilungsprojekte\eco\ResGroups\Narwani\Eawag\ChlamEE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeybernhardt/Documents/ChlamEE-TPC/data-general/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13845"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13840"/>
   </bookViews>
   <sheets>
     <sheet name="ChlamEE Treatments" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -75,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -218,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +404,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -559,10 +579,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -887,16 +911,16 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -911,7 +935,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -922,390 +946,393 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>34</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>8</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>11</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>21</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>35</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="24" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>13</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>16</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>18</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>26</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>3</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>6</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="2" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
         <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>32</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>33</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>35</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:D36">
+    <sortCondition ref="B2:B36"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>